<commit_message>
updated plot and outlier code
</commit_message>
<xml_diff>
--- a/T_SOL_summary.xlsx
+++ b/T_SOL_summary.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="720">
   <si>
     <t>Description</t>
   </si>
@@ -463,6 +463,1716 @@
   </si>
   <si>
     <t>-83.27 ± 97.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>39.62 ± 18.52</t>
+  </si>
+  <si>
+    <t>12.84 ± 63.88</t>
+  </si>
+  <si>
+    <t>52.97 ± 54.04</t>
+  </si>
+  <si>
+    <t>-47.16 ± 59.19</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>38.96 ± 19.56</t>
+  </si>
+  <si>
+    <t>51.85 ± 64.65</t>
+  </si>
+  <si>
+    <t>59.52 ± 54.27</t>
+  </si>
+  <si>
+    <t>-85.09 ± 68.88</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>31.45 ± 15.87</t>
+  </si>
+  <si>
+    <t>63.08 ± 65.10</t>
+  </si>
+  <si>
+    <t>65.37 ± 54.44</t>
+  </si>
+  <si>
+    <t>-76.21 ± 60.06</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>30.32 ± 14.14</t>
+  </si>
+  <si>
+    <t>-15.22 ± 24.18</t>
+  </si>
+  <si>
+    <t>52.51 ± 45.95</t>
+  </si>
+  <si>
+    <t>-18.29 ± 40.86</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>35.27 ± 17.72</t>
+  </si>
+  <si>
+    <t>29.82 ± 65.99</t>
+  </si>
+  <si>
+    <t>57.67 ± 52.86</t>
+  </si>
+  <si>
+    <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>44.57 ± 29.38</t>
+  </si>
+  <si>
+    <t>12.98 ± 70.52</t>
+  </si>
+  <si>
+    <t>67.04 ± 80.91</t>
+  </si>
+  <si>
+    <t>-62.06 ± 80.26</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>44.37 ± 31.01</t>
+  </si>
+  <si>
+    <t>53.26 ± 74.03</t>
+  </si>
+  <si>
+    <t>105.55 ± 120.63</t>
+  </si>
+  <si>
+    <t>-134.68 ± 110.16</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>36.81 ± 33.90</t>
+  </si>
+  <si>
+    <t>65.79 ± 84.67</t>
+  </si>
+  <si>
+    <t>88.54 ± 99.35</t>
+  </si>
+  <si>
+    <t>-96.48 ± 84.47</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>32.71 ± 22.29</t>
+  </si>
+  <si>
+    <t>-15.18 ± 26.14</t>
+  </si>
+  <si>
+    <t>62.16 ± 73.93</t>
+  </si>
+  <si>
+    <t>-24.29 ± 53.80</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>39.99 ± 30.32</t>
+  </si>
+  <si>
+    <t>31.48 ± 76.50</t>
+  </si>
+  <si>
+    <t>80.64 ± 96.44</t>
+  </si>
+  <si>
+    <t>-80.38 ± 92.78</t>
   </si>
 </sst>
 </file>
@@ -483,7 +2193,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -496,17 +2206,55 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,111 +2268,111 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="true"/>
-    <col min="2" max="2" width="13.140625" customWidth="true"/>
+    <col min="2" max="2" width="12.140625" customWidth="true"/>
     <col min="3" max="3" width="14.140625" customWidth="true"/>
-    <col min="4" max="4" width="13.140625" customWidth="true"/>
+    <col min="4" max="4" width="12.140625" customWidth="true"/>
     <col min="5" max="5" width="12.85546875" customWidth="true"/>
-    <col min="6" max="6" width="13.140625" customWidth="true"/>
+    <col min="6" max="6" width="12.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>120</v>
+        <v>690</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>125</v>
+        <v>695</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>130</v>
+        <v>700</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>135</v>
+        <v>705</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>140</v>
+        <v>710</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>145</v>
+        <v>715</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>121</v>
+        <v>691</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>126</v>
+        <v>696</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>131</v>
+        <v>701</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>136</v>
+        <v>706</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>141</v>
+        <v>711</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>146</v>
+        <v>716</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>122</v>
+        <v>692</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>127</v>
+        <v>697</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>132</v>
+        <v>702</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>137</v>
+        <v>707</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>142</v>
+        <v>712</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>147</v>
+        <v>717</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>123</v>
+        <v>693</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>128</v>
+        <v>698</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>133</v>
+        <v>703</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>138</v>
+        <v>708</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>143</v>
+        <v>713</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>148</v>
+        <v>718</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>124</v>
+        <v>694</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>129</v>
+        <v>699</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>134</v>
+        <v>704</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>139</v>
+        <v>709</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>144</v>
+        <v>714</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>149</v>
+        <v>719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Table 2 raw histograms (SOL)
</commit_message>
<xml_diff>
--- a/T_SOL_summary.xlsx
+++ b/T_SOL_summary.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="750">
   <si>
     <t>Description</t>
   </si>
@@ -2083,6 +2083,96 @@
   </si>
   <si>
     <t>-56.33 ± 62.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>44.57 ± 29.38</t>
+  </si>
+  <si>
+    <t>12.98 ± 70.52</t>
+  </si>
+  <si>
+    <t>67.04 ± 80.91</t>
+  </si>
+  <si>
+    <t>-62.06 ± 80.26</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>44.37 ± 31.01</t>
+  </si>
+  <si>
+    <t>53.26 ± 74.03</t>
+  </si>
+  <si>
+    <t>105.55 ± 120.63</t>
+  </si>
+  <si>
+    <t>-134.68 ± 110.16</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>36.81 ± 33.90</t>
+  </si>
+  <si>
+    <t>65.79 ± 84.67</t>
+  </si>
+  <si>
+    <t>88.54 ± 99.35</t>
+  </si>
+  <si>
+    <t>-96.48 ± 84.47</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>32.71 ± 22.29</t>
+  </si>
+  <si>
+    <t>-15.18 ± 26.14</t>
+  </si>
+  <si>
+    <t>62.16 ± 73.93</t>
+  </si>
+  <si>
+    <t>-24.29 ± 53.80</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>39.99 ± 30.32</t>
+  </si>
+  <si>
+    <t>31.48 ± 76.50</t>
+  </si>
+  <si>
+    <t>80.64 ± 96.44</t>
+  </si>
+  <si>
+    <t>-80.38 ± 92.78</t>
   </si>
   <si>
     <t>Description</t>
@@ -2193,7 +2283,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -2225,11 +2315,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -2255,6 +2346,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2277,102 +2369,102 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>690</v>
+        <v>720</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>695</v>
+        <v>725</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>700</v>
+        <v>730</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>705</v>
+        <v>735</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>710</v>
+        <v>740</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>715</v>
+        <v>745</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>691</v>
+        <v>721</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>696</v>
+        <v>726</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>701</v>
+        <v>731</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>706</v>
+        <v>736</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>711</v>
+        <v>741</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>716</v>
+        <v>746</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>692</v>
+        <v>722</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>697</v>
+        <v>727</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>702</v>
+        <v>732</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>707</v>
+        <v>737</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>712</v>
+        <v>742</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>717</v>
+        <v>747</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>693</v>
+        <v>723</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>698</v>
+        <v>728</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>703</v>
+        <v>733</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>708</v>
+        <v>738</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>713</v>
+        <v>743</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>718</v>
+        <v>748</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>694</v>
+        <v>724</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>699</v>
+        <v>729</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>704</v>
+        <v>734</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>709</v>
+        <v>739</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>714</v>
+        <v>744</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>719</v>
+        <v>749</v>
       </c>
     </row>
   </sheetData>

</xml_diff>